<commit_message>
Update Bug_Report_And_Test-case_Volvo Eicher Claim.xlsx
</commit_message>
<xml_diff>
--- a/Bug_Report_And_Test-case_Volvo Eicher Claim.xlsx
+++ b/Bug_Report_And_Test-case_Volvo Eicher Claim.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechFour\Documents\GitHub\Test-Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC992A1B-7F80-422C-88CA-C173F34611F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD218C6-0873-41C3-B9A8-4FF163BCF578}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11310" activeTab="2" xr2:uid="{71BF4958-A961-4E76-9BC7-C17C2F64A229}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11310" activeTab="1" xr2:uid="{71BF4958-A961-4E76-9BC7-C17C2F64A229}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="250">
   <si>
     <t xml:space="preserve">Bug Report </t>
   </si>
@@ -1700,7 +1700,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1800,6 +1800,15 @@
     <xf numFmtId="14" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1844,12 +1853,6 @@
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2184,18 +2187,18 @@
   </cols>
   <sheetData>
     <row r="8" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="42" t="s">
         <v>219</v>
       </c>
-      <c r="E8" s="40"/>
-      <c r="F8" s="41"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="44"/>
       <c r="G8" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="40" t="s">
         <v>229</v>
       </c>
-      <c r="I8" s="38"/>
+      <c r="I8" s="41"/>
     </row>
     <row r="9" spans="4:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D9" s="31" t="s">
@@ -2269,8 +2272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DBD0D03-4052-434A-81DB-12104B29E3C9}">
   <dimension ref="A1:PY56"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D5" sqref="A1:P56"/>
+    <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
+      <selection activeCell="L54" sqref="A1:P56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2293,45 +2296,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:441" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
     </row>
     <row r="2" spans="1:441" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="43" t="s">
+      <c r="B2" s="45"/>
+      <c r="C2" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="43"/>
+      <c r="D2" s="46"/>
       <c r="E2" s="34"/>
       <c r="F2" s="34"/>
       <c r="G2" s="34"/>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="44"/>
-      <c r="J2" s="45" t="s">
+      <c r="I2" s="47"/>
+      <c r="J2" s="48" t="s">
         <v>229</v>
       </c>
-      <c r="K2" s="45"/>
+      <c r="K2" s="48"/>
       <c r="L2" s="34"/>
       <c r="M2" s="33"/>
       <c r="N2" s="33"/>
@@ -2339,25 +2342,25 @@
       <c r="P2" s="33"/>
     </row>
     <row r="3" spans="1:441" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="43" t="s">
+      <c r="B3" s="45"/>
+      <c r="C3" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="43"/>
+      <c r="D3" s="46"/>
       <c r="E3" s="34"/>
       <c r="F3" s="34"/>
       <c r="G3" s="34"/>
-      <c r="H3" s="44" t="s">
+      <c r="H3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="44"/>
-      <c r="J3" s="45">
+      <c r="I3" s="47"/>
+      <c r="J3" s="48">
         <v>10008</v>
       </c>
-      <c r="K3" s="45"/>
+      <c r="K3" s="48"/>
       <c r="L3" s="34"/>
       <c r="M3" s="33"/>
       <c r="N3" s="33"/>
@@ -20316,8 +20319,8 @@
       <c r="J53" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="K53" s="33" t="s">
-        <v>29</v>
+      <c r="K53" s="36" t="s">
+        <v>64</v>
       </c>
       <c r="L53" s="33" t="s">
         <v>229</v>
@@ -20781,8 +20784,8 @@
       <c r="J54" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="K54" s="33" t="s">
-        <v>29</v>
+      <c r="K54" s="36" t="s">
+        <v>64</v>
       </c>
       <c r="L54" s="33" t="s">
         <v>229</v>
@@ -20795,7 +20798,7 @@
       <c r="P54" s="3"/>
     </row>
     <row r="55" spans="1:441" ht="60" x14ac:dyDescent="0.25">
-      <c r="A55" s="52">
+      <c r="A55" s="38">
         <v>43880</v>
       </c>
       <c r="B55" s="35" t="s">
@@ -20816,18 +20819,24 @@
       <c r="G55" s="33" t="s">
         <v>247</v>
       </c>
-      <c r="H55" s="53"/>
-      <c r="I55" s="53"/>
-      <c r="J55" s="53"/>
-      <c r="K55" s="53"/>
-      <c r="L55" s="53"/>
-      <c r="M55" s="53"/>
-      <c r="N55" s="53"/>
-      <c r="O55" s="53"/>
-      <c r="P55" s="53"/>
+      <c r="H55" s="39"/>
+      <c r="I55" s="39"/>
+      <c r="J55" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="K55" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="L55" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="M55" s="39"/>
+      <c r="N55" s="39"/>
+      <c r="O55" s="39"/>
+      <c r="P55" s="39"/>
     </row>
     <row r="56" spans="1:441" ht="60" x14ac:dyDescent="0.25">
-      <c r="A56" s="52">
+      <c r="A56" s="38">
         <v>43880</v>
       </c>
       <c r="B56" s="35" t="s">
@@ -20848,15 +20857,21 @@
       <c r="G56" s="33" t="s">
         <v>248</v>
       </c>
-      <c r="H56" s="53"/>
-      <c r="I56" s="53"/>
-      <c r="J56" s="53"/>
-      <c r="K56" s="53"/>
-      <c r="L56" s="53"/>
-      <c r="M56" s="53"/>
-      <c r="N56" s="53"/>
-      <c r="O56" s="53"/>
-      <c r="P56" s="53"/>
+      <c r="H56" s="39"/>
+      <c r="I56" s="39"/>
+      <c r="J56" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="K56" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="L56" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="M56" s="39"/>
+      <c r="N56" s="39"/>
+      <c r="O56" s="39"/>
+      <c r="P56" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -20908,7 +20923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02CF07D1-DB9D-46E0-8F35-4E41CC253122}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="C16" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -20926,15 +20941,15 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="20"/>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="52" t="s">
         <v>179</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
       <c r="I1" s="20"/>
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
@@ -20943,15 +20958,15 @@
       <c r="A2" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="50"/>
+      <c r="C2" s="53"/>
       <c r="D2" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
       <c r="G2" s="21" t="s">
         <v>182</v>
       </c>
@@ -20966,15 +20981,15 @@
       <c r="A3" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="B3" s="51">
+      <c r="B3" s="54">
         <v>43875</v>
       </c>
-      <c r="C3" s="51"/>
+      <c r="C3" s="54"/>
       <c r="D3" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
       <c r="G3" s="21" t="s">
         <v>186</v>
       </c>
@@ -20989,15 +21004,15 @@
       <c r="A4" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="51" t="s">
         <v>189</v>
       </c>
-      <c r="F4" s="48"/>
+      <c r="F4" s="51"/>
       <c r="G4" s="21" t="s">
         <v>190</v>
       </c>

</xml_diff>